<commit_message>
chore: 재고 관리 대장 template 수정
- 전극
- 조립
</commit_message>
<xml_diff>
--- a/data/templates/electrode.xlsx
+++ b/data/templates/electrode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7556226-6F69-4158-9B2B-F36F948B2403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7432E6-F90C-402E-8D5A-FD7244326901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1365" windowWidth="19005" windowHeight="11460" xr2:uid="{FF53B2FD-47B5-4C34-8976-0E8A1B40CF6E}"/>
+    <workbookView xWindow="1740" yWindow="1605" windowWidth="19005" windowHeight="11460" xr2:uid="{FF53B2FD-47B5-4C34-8976-0E8A1B40CF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="전극" sheetId="1" r:id="rId1"/>
@@ -599,7 +599,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -651,9 +651,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,12 +702,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -753,6 +744,22 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="쉼표 [0] 2" xfId="2" xr:uid="{4E413DB9-CD7D-4626-9908-0F49E1498519}"/>
@@ -1152,244 +1159,244 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.875" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.25" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.875" style="27" customWidth="1"/>
     <col min="10" max="10" width="5" style="5" customWidth="1"/>
     <col min="11" max="11" width="9.125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.625" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.625" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="57" customWidth="1"/>
     <col min="14" max="14" width="5.125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="27"/>
+      <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:14" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="25"/>
+    <row r="2" spans="1:14" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="24"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="14"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="36"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="35"/>
       <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="40"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
       <c r="E4" s="12"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="36"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="35"/>
       <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="40"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="12"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="34"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
       <c r="K5" s="16"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="36"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="35"/>
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="40"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="12"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
       <c r="K6" s="16"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="36"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="35"/>
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="12"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="35"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="14"/>
       <c r="J7" s="11"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="36"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="15"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
       <c r="E8" s="12"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="35"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="14"/>
       <c r="J8" s="11"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="36"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="35"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="18"/>
       <c r="D9" s="17"/>
       <c r="E9" s="12"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="35"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="14"/>
       <c r="J9" s="11"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="36"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="15"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="18"/>
       <c r="D10" s="17"/>
       <c r="E10" s="12"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="35"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="14"/>
       <c r="J10" s="11"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="36"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="18"/>
       <c r="D11" s="17"/>
       <c r="E11" s="12"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="35"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="14"/>
       <c r="J11" s="11"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="36"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="18"/>
       <c r="D12" s="17"/>
       <c r="E12" s="12"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="35"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="14"/>
       <c r="J12" s="11"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="36"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="35"/>
       <c r="N12" s="15"/>
     </row>
   </sheetData>

</xml_diff>